<commit_message>
Need to compress CovMatrix. Finished optimization w/out correlation
</commit_message>
<xml_diff>
--- a/FinalProject/Analysis_Carpenter/Example Functions/Example of Calculations.xlsx
+++ b/FinalProject/Analysis_Carpenter/Example Functions/Example of Calculations.xlsx
@@ -8,13 +8,48 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive\Documents\DScourseS20\FinalProject\Analysis_Carpenter\Example Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B838144-FEB5-4A09-8219-B45B008EDC5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53EB394-73FC-44AD-9B8C-3EEF19FE1F09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22597" yWindow="-3773" windowWidth="22695" windowHeight="14596" xr2:uid="{01243FC1-56D7-4640-8CA6-0969CF9A54A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Calcs" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Calcs!$C$15:$G$15</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Calcs!$C$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Calcs!$H$15</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Calcs!$C$3</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0.05</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterate="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -711,7 +746,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +769,7 @@
       </c>
       <c r="C3" s="22">
         <f t="array" ref="C3">SQRT(MMULT(MMULT(C15:G15,C20:G24),TRANSPOSE(C15:G15)))</f>
-        <v>0.33247101305895294</v>
+        <v>0.22382297157025347</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>15</v>
@@ -769,7 +804,7 @@
       </c>
       <c r="C6" s="22">
         <f t="array" ref="C6">MMULT(C15:G15,TRANSPOSE(C26:G26))</f>
-        <v>0.29213073470380935</v>
+        <v>5.0000000878243675E-2</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>15</v>
@@ -804,7 +839,7 @@
       </c>
       <c r="C9" s="19">
         <f>(C6-C10)/C3</f>
-        <v>0.81850965652622409</v>
+        <v>0.13403450355330165</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" t="s">
@@ -867,23 +902,23 @@
         <v>7</v>
       </c>
       <c r="C15" s="11">
-        <v>6.1520041272871327E-2</v>
+        <v>0</v>
       </c>
       <c r="D15" s="11">
         <v>0</v>
       </c>
       <c r="E15" s="11">
-        <v>0</v>
+        <v>0.41085053811994493</v>
       </c>
       <c r="F15" s="11">
-        <v>0.48434121260564111</v>
+        <v>-4.8434121259268236E-7</v>
       </c>
       <c r="G15" s="11">
-        <v>0.45413874357388551</v>
+        <v>0.58914993859401388</v>
       </c>
       <c r="H15" s="10">
         <f>SUM(C15:G15)</f>
-        <v>0.99999999745239798</v>
+        <v>0.99999999237274628</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Attempt New Optimization Calc
</commit_message>
<xml_diff>
--- a/FinalProject/Analysis_Carpenter/Example Functions/Example of Calculations.xlsx
+++ b/FinalProject/Analysis_Carpenter/Example Functions/Example of Calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive\Documents\DScourseS20\FinalProject\Analysis_Carpenter\Example Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53EB394-73FC-44AD-9B8C-3EEF19FE1F09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CA8D05-6282-49AD-ADD5-A2281A7237EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22597" yWindow="-3773" windowWidth="22695" windowHeight="14596" xr2:uid="{01243FC1-56D7-4640-8CA6-0969CF9A54A6}"/>
   </bookViews>
@@ -746,7 +746,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>